<commit_message>
feat: add Client, Type, and Companies House Number to buildings
Added three new columns to buildings import:
- Client: Management company/client name
- Type: Building ownership type (RMC, RTM, Freehold, Leasehold)
- Companies House Number: Registration number for RMC/RTM

Changes:
- Updated Excel template with new columns and example data
- Updated import script to handle new fields
- Created database migration to add columns
- Added indexes for client and companies house number lookup

Example data shows RMC structure with Companies House number.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/BlocIQ_Onboarding_Template.xlsx
+++ b/BlocIQ_Onboarding_Template.xlsx
@@ -17,11 +17,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="216">
   <si>
     <t>Building Name*</t>
   </si>
   <si>
+    <t>Client*</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Companies House Number</t>
+  </si>
+  <si>
     <t>Address*</t>
   </si>
   <si>
@@ -67,6 +76,15 @@
     <t>Example Court</t>
   </si>
   <si>
+    <t>Pimlico Place Management Company Limited</t>
+  </si>
+  <si>
+    <t>RMC</t>
+  </si>
+  <si>
+    <t>3805608</t>
+  </si>
+  <si>
     <t>123 Example Street, London</t>
   </si>
   <si>
@@ -95,6 +113,9 @@
   </si>
   <si>
     <t>INSTRUCTIONS: Fill in one row per building. Fields marked with * are required.</t>
+  </si>
+  <si>
+    <t>Type options: RMC (Resident Management Company), RTM (Right to Manage), Freehold, Leasehold</t>
   </si>
   <si>
     <t>Building Type options: residential, commercial, mixed_use</t>
@@ -1102,26 +1123,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:R6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="40" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="10" max="10" width="30" customWidth="1"/>
-    <col min="11" max="11" width="40" customWidth="1"/>
-    <col min="12" max="13" width="25" customWidth="1"/>
-    <col min="14" max="14" width="22" customWidth="1"/>
-    <col min="15" max="15" width="50" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="12" max="12" width="22" customWidth="1"/>
+    <col min="13" max="13" width="30" customWidth="1"/>
+    <col min="14" max="14" width="40" customWidth="1"/>
+    <col min="15" max="16" width="25" customWidth="1"/>
+    <col min="17" max="17" width="22" customWidth="1"/>
+    <col min="18" max="18" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1167,67 +1191,90 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2">
         <v>1990</v>
       </c>
-      <c r="G2">
+      <c r="J2">
         <v>5</v>
       </c>
-      <c r="H2">
+      <c r="K2">
         <v>24</v>
       </c>
-      <c r="I2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2">
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2">
         <v>120000</v>
       </c>
-      <c r="M2">
+      <c r="P2">
         <v>50000</v>
       </c>
-      <c r="N2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" t="s">
-        <v>24</v>
+      <c r="Q2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1259,63 +1306,63 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1327,16 +1374,16 @@
         <v>750</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="K2" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="L2">
         <v>250</v>
@@ -1345,27 +1392,27 @@
         <v>2400</v>
       </c>
       <c r="N2" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="O2" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="P2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" t="s">
         <v>52</v>
-      </c>
-      <c r="D3" t="s">
-        <v>45</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1377,16 +1424,16 @@
         <v>550</v>
       </c>
       <c r="H3" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="K3" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="L3">
         <v>250</v>
@@ -1395,23 +1442,23 @@
         <v>1800</v>
       </c>
       <c r="N3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="O3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="P3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1448,195 +1495,195 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="H2" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="I2" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="J2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="K2" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="L2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="M2" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="N2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="O2" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="P2" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="Q2" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="R2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="S2" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="T2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="E3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J3" t="s">
+        <v>96</v>
+      </c>
+      <c r="K3" t="s">
+        <v>97</v>
+      </c>
+      <c r="L3" t="s">
+        <v>98</v>
+      </c>
+      <c r="M3" t="s">
         <v>86</v>
       </c>
-      <c r="F3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" t="s">
-        <v>88</v>
-      </c>
-      <c r="J3" t="s">
-        <v>89</v>
-      </c>
-      <c r="K3" t="s">
-        <v>90</v>
-      </c>
-      <c r="L3" t="s">
-        <v>91</v>
-      </c>
-      <c r="M3" t="s">
-        <v>79</v>
-      </c>
       <c r="N3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="O3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="P3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="Q3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="R3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="S3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="T3" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1670,72 +1717,72 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="F2">
         <v>125</v>
@@ -1747,7 +1794,7 @@
         <v>250</v>
       </c>
       <c r="I2" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="J2">
         <v>25</v>
@@ -1759,39 +1806,39 @@
         <v>250000</v>
       </c>
       <c r="M2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="N2" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="O2" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="P2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="Q2" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="R2" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="F3">
         <v>125</v>
@@ -1803,7 +1850,7 @@
         <v>250</v>
       </c>
       <c r="I3" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="J3">
         <v>25</v>
@@ -1815,32 +1862,32 @@
         <v>180000</v>
       </c>
       <c r="M3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="N3" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="O3" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="P3" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="Q3" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="R3" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1868,164 +1915,164 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="D2">
         <v>4.17</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="H2" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="I2" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D3">
         <v>4.17</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="H3" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="I3" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="D4">
         <v>3.13</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="H4" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="I4" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D5">
         <v>3.13</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="H5" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="I5" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2055,154 +2102,154 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C2" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="D2" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="E2" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="F2" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="G2" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="H2" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="I2" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="J2">
         <v>850</v>
       </c>
       <c r="K2" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C3" t="s">
         <v>149</v>
       </c>
-      <c r="C3" t="s">
-        <v>142</v>
-      </c>
       <c r="D3" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="E3" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="F3" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="G3" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="H3" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="I3" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="J3">
         <v>1200</v>
       </c>
       <c r="K3" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="C4" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="D4" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="E4" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="F4" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="G4" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="H4" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="I4" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="J4">
         <v>450</v>
       </c>
       <c r="K4" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2221,257 +2268,257 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>